<commit_message>
PPT distintas vistas, actu niko nikos y video muestra
</commit_message>
<xml_diff>
--- a/Sprint 2/Calendario Nikonikos.xlsx
+++ b/Sprint 2/Calendario Nikonikos.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="19440" windowHeight="8010"/>
   </bookViews>
@@ -42,8 +47,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +116,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2768,6 +2781,290 @@
         <a:xfrm>
           <a:off x="7143750" y="4543425"/>
           <a:ext cx="333374" cy="333374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>596900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="3822700"/>
+          <a:ext cx="558800" cy="558800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>584200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="82" name="Imagen 81"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10960100" y="3810000"/>
+          <a:ext cx="558800" cy="558800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>573984</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>600075</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="83" name="15 Imagen" descr="Feliz.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7543800" y="3784600"/>
+          <a:ext cx="573984" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>573984</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>600075</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="84" name="15 Imagen" descr="Feliz.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="3784600"/>
+          <a:ext cx="573984" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>596900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagen 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9271000" y="3810000"/>
+          <a:ext cx="571500" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>573984</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>600075</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="86" name="15 Imagen" descr="Feliz.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12573000" y="3784600"/>
+          <a:ext cx="573984" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>568325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="87" name="73 Imagen" descr="Dormido.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11811000" y="3848100"/>
+          <a:ext cx="504825" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2822,7 +3119,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2854,9 +3151,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2888,6 +3203,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3063,17 +3396,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>42654</v>
       </c>
@@ -3120,7 +3453,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="4" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -3140,7 +3473,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="5" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -3160,7 +3493,7 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="6" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -3180,7 +3513,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="7" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -3200,7 +3533,7 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="8" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -3220,7 +3553,7 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="9" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -3240,7 +3573,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="10" spans="1:16" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -3260,7 +3593,7 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:16" ht="15.75" thickTop="1"/>
+    <row r="11" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3269,24 +3602,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>